<commit_message>
* Reworked the parser to be more object based * Removed passing around tokens in many places (still have a lot of them around though). * Location information moved into a standalone object so it can be more easily passed around.
</commit_message>
<xml_diff>
--- a/Tools/Z80 Opcodes.xlsx
+++ b/Tools/Z80 Opcodes.xlsx
@@ -1304,8 +1304,8 @@
   <dimension ref="A1:T843"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F765" sqref="F765"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>